<commit_message>
Added cooking and logs directories in bbq
</commit_message>
<xml_diff>
--- a/bbq-stuff/logs/pulled-pork-may-2019.xlsx
+++ b/bbq-stuff/logs/pulled-pork-may-2019.xlsx
@@ -24,12 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Plateau was longer than necessary due to dome temp drop between 6:30 and 9:30</t>
   </si>
   <si>
     <t>Target temp 195 from beginning until 15:21</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Minute</t>
+  </si>
+  <si>
+    <t>Total Minutes</t>
+  </si>
+  <si>
+    <t>Meat Temp</t>
+  </si>
+  <si>
+    <t>Dome Temp (analog)</t>
+  </si>
+  <si>
+    <t>7.8 lb Boston butt bone in</t>
   </si>
 </sst>
 </file>
@@ -153,7 +171,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$37</c:f>
+              <c:f>Sheet1!$C$2:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="37"/>
@@ -237,7 +255,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$37</c:f>
+              <c:f>Sheet1!$D$2:$D$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -338,7 +356,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$37</c:f>
+              <c:f>Sheet1!$C$2:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="37"/>
@@ -422,7 +440,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$1:$E$37</c:f>
+              <c:f>Sheet1!$E$2:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="37"/>
@@ -515,11 +533,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="236473184"/>
-        <c:axId val="236474360"/>
+        <c:axId val="216640808"/>
+        <c:axId val="216641192"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="236473184"/>
+        <c:axId val="216640808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -562,14 +580,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236474360"/>
+        <c:crossAx val="216641192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="236474360"/>
+        <c:axId val="216641192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="50"/>
@@ -621,7 +639,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236473184"/>
+        <c:crossAx val="216640808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1232,13 +1250,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>4761</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1524,48 +1542,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <f>(A1*60)+B1</f>
-        <v>0</v>
-      </c>
-      <c r="D1">
-        <v>41</v>
-      </c>
-      <c r="E1">
-        <v>190</v>
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C25" si="0">(A2*60)+B2</f>
-        <v>60</v>
+        <f>(A2*60)+B2</f>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>190</v>
@@ -1576,17 +1597,17 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" si="0"/>
-        <v>72</v>
+        <f t="shared" ref="C3:C26" si="0">(A3*60)+B3</f>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>58.5</v>
+        <v>52</v>
       </c>
       <c r="E3">
-        <v>175</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1594,17 +1615,17 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D4">
-        <v>64</v>
+        <v>58.5</v>
       </c>
       <c r="E4">
-        <v>185</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1612,17 +1633,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="1">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D5">
-        <v>72.5</v>
+        <v>64</v>
       </c>
       <c r="E5">
-        <v>195</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1630,71 +1651,71 @@
         <v>1</v>
       </c>
       <c r="B6" s="1">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D6">
-        <v>80.400000000000006</v>
+        <v>72.5</v>
       </c>
       <c r="E6">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>387</v>
+        <v>117</v>
       </c>
       <c r="D7">
-        <v>136.5</v>
+        <v>80.400000000000006</v>
       </c>
       <c r="E7">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>570</v>
+        <v>387</v>
       </c>
       <c r="D8">
-        <v>147</v>
+        <v>136.5</v>
       </c>
       <c r="E8">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>614</v>
+        <v>570</v>
       </c>
       <c r="D9">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9">
-        <v>190</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1702,17 +1723,17 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>632</v>
+        <v>614</v>
       </c>
       <c r="D10">
-        <v>149.5</v>
+        <v>148</v>
       </c>
       <c r="E10">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,89 +1741,89 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>640</v>
+        <v>632</v>
       </c>
       <c r="D11">
-        <v>150</v>
+        <v>149.5</v>
       </c>
       <c r="E11">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>677</v>
+        <v>640</v>
       </c>
       <c r="D12">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E12">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>732</v>
+        <v>677</v>
       </c>
       <c r="D13">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="E13">
-        <v>210</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>797</v>
+        <v>732</v>
       </c>
       <c r="D14">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E14">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>841</v>
+        <v>797</v>
       </c>
       <c r="D15">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E15">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1810,32 +1831,32 @@
         <v>14</v>
       </c>
       <c r="B16" s="1">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>892</v>
+        <v>841</v>
       </c>
       <c r="D16">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E16">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="1">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>910</v>
+        <v>892</v>
       </c>
       <c r="D17">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E17">
         <v>185</v>
@@ -1846,17 +1867,17 @@
         <v>15</v>
       </c>
       <c r="B18" s="1">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>921</v>
+        <v>910</v>
       </c>
       <c r="D18">
         <v>167</v>
       </c>
       <c r="E18">
-        <v>220</v>
+        <v>185</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1864,17 +1885,17 @@
         <v>15</v>
       </c>
       <c r="B19" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
-        <v>925</v>
+        <v>921</v>
       </c>
       <c r="D19">
-        <v>166.6</v>
+        <v>167</v>
       </c>
       <c r="E19">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1882,17 +1903,17 @@
         <v>15</v>
       </c>
       <c r="B20" s="1">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>948</v>
+        <v>925</v>
       </c>
       <c r="D20">
-        <v>170</v>
-      </c>
-      <c r="E20" s="1">
-        <v>240</v>
+        <v>166.6</v>
+      </c>
+      <c r="E20">
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1900,34 +1921,34 @@
         <v>15</v>
       </c>
       <c r="B21" s="1">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="D21">
-        <v>171</v>
-      </c>
-      <c r="E21">
-        <v>245</v>
+        <v>170</v>
+      </c>
+      <c r="E21" s="1">
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" s="1">
-        <v>7</v>
+        <v>56</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>967</v>
+        <v>956</v>
       </c>
       <c r="D22">
-        <v>173</v>
-      </c>
-      <c r="E22" s="1">
+        <v>171</v>
+      </c>
+      <c r="E22">
         <v>245</v>
       </c>
     </row>
@@ -1936,62 +1957,85 @@
         <v>16</v>
       </c>
       <c r="B23" s="1">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>989</v>
+        <v>967</v>
       </c>
       <c r="D23">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E23" s="1">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="1">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>1046</v>
+        <v>989</v>
       </c>
       <c r="D24">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="E24" s="1">
-        <v>240</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>1080</v>
+        <v>1046</v>
       </c>
       <c r="D25">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E25" s="1">
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>1080</v>
+      </c>
+      <c r="D26">
+        <v>191</v>
+      </c>
+      <c r="E26" s="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>